<commit_message>
add single store report template
</commit_message>
<xml_diff>
--- a/reports/templates/daily.xlsx
+++ b/reports/templates/daily.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uicestone/Sites/minimars-server/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0C1353-06F6-8B40-B592-8710C43737DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358903ED-9225-A243-BDA1-B77C97F61251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="1000" windowWidth="26840" windowHeight="16440" xr2:uid="{4F58C902-78D5-2145-A3CE-3267BB3BABFE}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
-  <si>
-    <t>门店</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="145">
   <si>
     <t>天山店</t>
   </si>
@@ -452,18 +449,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>票务订单数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>${TS_guestPlayAmount}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>散客+平台订单收款（未使用卡和余额支付的订单）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>仅自营次卡</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -484,7 +473,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>散客办卡口径待确认</t>
+    <t>餐饮销售额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${TS_foodSalesAmount}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${JN_foodSalesAmount}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${HX_foodSalesAmount}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${BY_foodSalesAmount}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${DY_foodSalesAmount}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -900,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8EA64C-3023-A04F-8D77-D73A58D0B3BC}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:F38"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -913,7 +922,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21">
       <c r="A1" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -922,97 +931,90 @@
       <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
       <c r="G2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>134</v>
-      </c>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>136</v>
-      </c>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="e">
         <f t="shared" ref="B6:F6" si="0">B7+B8+B9</f>
@@ -1037,299 +1039,309 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>139</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="7" t="e">
-        <f>B14/(B12+B14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C13" s="7" t="e">
-        <f>C14/(C12+C14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" s="7" t="e">
-        <f>D14/(D12+D14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E13" s="7" t="e">
-        <f t="shared" ref="E13:F13" si="1">E14/(E12+E14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F13" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>142</v>
+        <v>8</v>
+      </c>
+      <c r="B14" s="7" t="e">
+        <f>B15/(B13+B15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C14" s="7" t="e">
+        <f>C15/(C13+C15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" s="7" t="e">
+        <f>D15/(D13+D15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" s="7" t="e">
+        <f t="shared" ref="E14:F14" si="1">E15/(E13+E15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F14" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="e">
-        <f t="shared" ref="B18:F18" si="2">B19+B20+B21+B24+B28+B29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C18" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D18" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E18" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>139</v>
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="e">
+        <f t="shared" ref="B19:F19" si="2">B20+B21+B22+B25+B29+B30</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C19" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1339,37 +1351,37 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>118</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1379,7 +1391,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1389,7 +1401,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1399,7 +1411,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1407,212 +1419,222 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="6" t="e">
-        <f>B33/B3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C31" s="6" t="e">
-        <f>C33/C3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D31" s="6" t="e">
-        <f>D33/D3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E31" s="6" t="e">
-        <f>E33/E3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F31" s="6" t="e">
-        <f>F33/F3</f>
-        <v>#VALUE!</v>
-      </c>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>123</v>
+        <v>24</v>
+      </c>
+      <c r="B32" s="6" t="e">
+        <f>B34/B3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C32" s="6" t="e">
+        <f>C34/C3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D32" s="6" t="e">
+        <f>D34/D3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E32" s="6" t="e">
+        <f>E34/E3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F32" s="6" t="e">
+        <f>F34/F3</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>128</v>
+        <v>25</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="7" t="e">
-        <f>B34/B33</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C35" s="7" t="e">
-        <f>C34/C33</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D35" s="7" t="e">
-        <f>D34/D33</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E35" s="7" t="e">
-        <f>E34/E33</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F35" s="7" t="e">
-        <f>F34/F33</f>
-        <v>#VALUE!</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" t="s">
-        <v>141</v>
+        <v>28</v>
+      </c>
+      <c r="B36" s="7" t="e">
+        <f>B35/B34</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C36" s="7" t="e">
+        <f>C35/C34</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D36" s="7" t="e">
+        <f>D35/D34</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E36" s="7" t="e">
+        <f>E35/E34</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F36" s="7" t="e">
+        <f>F35/F34</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="7" t="e">
-        <f>B36/B33</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C38" s="7" t="e">
-        <f t="shared" ref="C38:F38" si="3">C36/C33</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D38" s="7" t="e">
+        <v>30</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="7" t="e">
+        <f>B37/B34</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C39" s="7" t="e">
+        <f t="shared" ref="C39:F39" si="3">C37/C34</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D39" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E38" s="7" t="e">
+      <c r="E39" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F38" s="7" t="e">
+      <c r="F39" s="7" t="e">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="7" t="e">
-        <f>B42/B3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C41" s="7" t="e">
-        <f t="shared" ref="C41:F41" si="4">C42/C3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D41" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E41" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F41" s="7" t="e">
-        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="7" t="e">
+        <f>B43/B3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C42" s="7" t="e">
+        <f>C43/C3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D42" s="7" t="e">
+        <f>D43/D3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E42" s="7" t="e">
+        <f>E43/E3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F42" s="7" t="e">
+        <f>F43/F3</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>